<commit_message>
Frontend changes and excel sheet changes
</commit_message>
<xml_diff>
--- a/backend/assets/timetables.xlsx
+++ b/backend/assets/timetables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ARAPP\NaviGo\backend\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8306F6-B095-4CED-BF8A-DB1278ECB1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611D885F-B02E-482C-A0DB-62928B35ADCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="102">
   <si>
     <t>Faculty</t>
   </si>
@@ -34,15 +34,6 @@
     <t>Mon 11:30-12:30</t>
   </si>
   <si>
-    <t>Mon 12:30-1:30</t>
-  </si>
-  <si>
-    <t>Mon 2:30-3:30</t>
-  </si>
-  <si>
-    <t>Mon 3:30-4:30</t>
-  </si>
-  <si>
     <t>Tue 9:00-10:00</t>
   </si>
   <si>
@@ -52,15 +43,6 @@
     <t>Tue 11:30-12:30</t>
   </si>
   <si>
-    <t>Tue 12:30-1:30</t>
-  </si>
-  <si>
-    <t>Tue 2:30-3:30</t>
-  </si>
-  <si>
-    <t>Tue 3:30-4:30</t>
-  </si>
-  <si>
     <t>Wed 9:00-10:00</t>
   </si>
   <si>
@@ -73,12 +55,6 @@
     <t>Wed 12:30-1:30</t>
   </si>
   <si>
-    <t>Wed 2:30-3:30</t>
-  </si>
-  <si>
-    <t>Wed 3:30-4:30</t>
-  </si>
-  <si>
     <t>Thu 9:00-10:00</t>
   </si>
   <si>
@@ -88,15 +64,6 @@
     <t>Thu 11:30-12:30</t>
   </si>
   <si>
-    <t>Thu 12:30-1:30</t>
-  </si>
-  <si>
-    <t>Thu 2:30-3:30</t>
-  </si>
-  <si>
-    <t>Thu 3:30-4:30</t>
-  </si>
-  <si>
     <t>Fri 9:00-10:00</t>
   </si>
   <si>
@@ -106,63 +73,6 @@
     <t>Fri 11:30-12:30</t>
   </si>
   <si>
-    <t>Fri 12:30-1:30</t>
-  </si>
-  <si>
-    <t>Fri 2:30-3:30</t>
-  </si>
-  <si>
-    <t>Fri 3:30-4:30</t>
-  </si>
-  <si>
-    <t>Unnamed: 31</t>
-  </si>
-  <si>
-    <t>Unnamed: 32</t>
-  </si>
-  <si>
-    <t>Unnamed: 33</t>
-  </si>
-  <si>
-    <t>Unnamed: 34</t>
-  </si>
-  <si>
-    <t>Unnamed: 35</t>
-  </si>
-  <si>
-    <t>Unnamed: 36</t>
-  </si>
-  <si>
-    <t>Unnamed: 37</t>
-  </si>
-  <si>
-    <t>Unnamed: 38</t>
-  </si>
-  <si>
-    <t>Unnamed: 39</t>
-  </si>
-  <si>
-    <t>Unnamed: 40</t>
-  </si>
-  <si>
-    <t>Unnamed: 41</t>
-  </si>
-  <si>
-    <t>Unnamed: 42</t>
-  </si>
-  <si>
-    <t>Unnamed: 43</t>
-  </si>
-  <si>
-    <t>Unnamed: 44</t>
-  </si>
-  <si>
-    <t>Unnamed: 45</t>
-  </si>
-  <si>
-    <t>Unnamed: 46</t>
-  </si>
-  <si>
     <t>Mrs. Padmavathi</t>
   </si>
   <si>
@@ -199,12 +109,6 @@
     <t>Mr. Joyan Prajwal Alvares</t>
   </si>
   <si>
-    <t>Mr.Manoj Sogi</t>
-  </si>
-  <si>
-    <t>Mrs.Divyashree M S</t>
-  </si>
-  <si>
     <t>Dr. B.R Vatsala</t>
   </si>
   <si>
@@ -334,9 +238,6 @@
     <t>CSLAB-8</t>
   </si>
   <si>
-    <t>CSLAB-5</t>
-  </si>
-  <si>
     <t>MB-3</t>
   </si>
   <si>
@@ -377,6 +278,54 @@
   </si>
   <si>
     <t>Ms. Sneha S</t>
+  </si>
+  <si>
+    <t>Mrs. Divyashree M S</t>
+  </si>
+  <si>
+    <t>Mr. Manoj Sogi</t>
+  </si>
+  <si>
+    <t>Thu 12:30-13:30</t>
+  </si>
+  <si>
+    <t>Thu 14:30-15:30</t>
+  </si>
+  <si>
+    <t>Mon 12:30-13:30</t>
+  </si>
+  <si>
+    <t>Mon 14:30-15:30</t>
+  </si>
+  <si>
+    <t>Mon 15:30-16:30</t>
+  </si>
+  <si>
+    <t>Tue 12:30-13:30</t>
+  </si>
+  <si>
+    <t>Tue 14:30-15:30</t>
+  </si>
+  <si>
+    <t>Tue 15:30-16:30</t>
+  </si>
+  <si>
+    <t>Wed 14:30-15:30</t>
+  </si>
+  <si>
+    <t>Wed 15:30-16:30</t>
+  </si>
+  <si>
+    <t>Thu 15:30-16:30</t>
+  </si>
+  <si>
+    <t>Fri 14:30-15:30</t>
+  </si>
+  <si>
+    <t>Fri 12:30-13:30</t>
+  </si>
+  <si>
+    <t>Fri 15:30-16:30</t>
   </si>
 </sst>
 </file>
@@ -746,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,9 +711,29 @@
     <col min="8" max="8" width="21.109375" customWidth="1"/>
     <col min="9" max="9" width="19.88671875" customWidth="1"/>
     <col min="10" max="10" width="17.44140625" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
     <col min="14" max="14" width="17.109375" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" customWidth="1"/>
+    <col min="18" max="18" width="20.5546875" customWidth="1"/>
+    <col min="19" max="19" width="16.33203125" customWidth="1"/>
+    <col min="20" max="20" width="18.33203125" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15" customWidth="1"/>
+    <col min="24" max="24" width="14.44140625" customWidth="1"/>
+    <col min="25" max="25" width="15.33203125" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" customWidth="1"/>
+    <col min="27" max="27" width="13.88671875" customWidth="1"/>
+    <col min="28" max="28" width="17.33203125" customWidth="1"/>
+    <col min="29" max="29" width="14.109375" customWidth="1"/>
+    <col min="30" max="30" width="22.33203125" customWidth="1"/>
+    <col min="31" max="31" width="22.88671875" customWidth="1"/>
+    <col min="32" max="32" width="17" customWidth="1"/>
+    <col min="33" max="33" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.3">
@@ -781,258 +750,220 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="AC1" s="1" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="J2">
         <v>203</v>
       </c>
       <c r="M2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="R2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="T2">
         <v>204</v>
       </c>
       <c r="V2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="X2" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Z2">
         <v>203</v>
       </c>
       <c r="AD2" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>302</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="G3">
         <v>401</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="AA3" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="AD3">
         <v>201</v>
       </c>
-      <c r="AF3">
-        <v>201</v>
-      </c>
-      <c r="AG3">
-        <v>201</v>
-      </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>301</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="H4">
         <v>301</v>
       </c>
       <c r="M4" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="P4">
         <v>301</v>
       </c>
       <c r="V4" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="X4" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="Y4" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="Z4" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="H5">
         <v>302</v>
@@ -1041,48 +972,48 @@
         <v>302</v>
       </c>
       <c r="M5" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O5" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="U5" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V5" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W5" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y5" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="Z5" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="AB5" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="AC5" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="AD5" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="G6">
         <v>401</v>
@@ -1091,36 +1022,36 @@
         <v>401</v>
       </c>
       <c r="U6" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V6" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W6" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="X6" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Z6" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="AA6" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="AB6" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="AD6" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="H7">
         <v>303</v>
@@ -1132,16 +1063,16 @@
         <v>303</v>
       </c>
       <c r="S7" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="T7" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="U7" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V7" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W7">
         <v>309</v>
@@ -1153,18 +1084,18 @@
         <v>309</v>
       </c>
       <c r="AA7" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="AB7" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="AC7" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="AA8">
         <v>108</v>
@@ -1178,28 +1109,10 @@
       <c r="AE8">
         <v>108</v>
       </c>
-      <c r="AF8">
-        <v>108</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>202</v>
@@ -1208,48 +1121,48 @@
         <v>302</v>
       </c>
       <c r="L9" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M9" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="T9" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="U9" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V9" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W9" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="AB9" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="AC9" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="U10" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V10" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W10" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="X10" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y10">
         <v>309</v>
@@ -1261,24 +1174,12 @@
         <v>309</v>
       </c>
       <c r="AD10" t="s">
-        <v>113</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="B11">
         <v>203</v>
@@ -1287,39 +1188,36 @@
         <v>203</v>
       </c>
       <c r="O11" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P11" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q11" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W11">
         <v>307</v>
       </c>
       <c r="AC11" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="AD11" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="AE11" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="J12" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="V12" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="AB12">
         <v>101</v>
@@ -1330,31 +1228,16 @@
       <c r="AE12">
         <v>101</v>
       </c>
-      <c r="AF12">
-        <v>201</v>
-      </c>
-      <c r="AH12">
-        <v>201</v>
-      </c>
-      <c r="AI12">
-        <v>201</v>
-      </c>
-      <c r="AJ12">
-        <v>201</v>
-      </c>
-      <c r="AK12">
-        <v>201</v>
-      </c>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>301</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="G13">
         <v>301</v>
@@ -1363,13 +1246,13 @@
         <v>301</v>
       </c>
       <c r="I13" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="L13" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="N13" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="P13">
         <v>301</v>
@@ -1378,39 +1261,39 @@
         <v>301</v>
       </c>
       <c r="W13" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="X13" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y13" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Z13" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="AB13">
         <v>308</v>
       </c>
       <c r="AD13" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="J14" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L14" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M14" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="S14">
         <v>304</v>
@@ -1427,7 +1310,7 @@
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="X15">
         <v>305</v>
@@ -1450,36 +1333,36 @@
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="J16" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K16" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L16" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M16" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O16" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P16" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>202</v>
@@ -1488,130 +1371,130 @@
         <v>203</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="G17" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="H17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="J17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O17" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="R18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="S18" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="T18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="J19" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K19" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L19" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M19" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N19" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="X19" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="Z19" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="AA19" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="AB19" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="AC19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="M20" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N20" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O20" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P20" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y20">
         <v>107</v>
@@ -1629,9 +1512,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="X21">
         <v>305</v>
@@ -1652,9 +1535,9 @@
         <v>306</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>202</v>
@@ -1669,10 +1552,10 @@
         <v>401</v>
       </c>
       <c r="L22" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M22" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q22">
         <v>202</v>
@@ -1684,9 +1567,9 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="I23">
         <v>302</v>
@@ -1701,15 +1584,15 @@
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="H24" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="I24">
         <v>303</v>
@@ -1718,7 +1601,7 @@
         <v>303</v>
       </c>
       <c r="P24" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="R24">
         <v>303</v>
@@ -1736,33 +1619,33 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="N25" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="P25">
         <v>301</v>
       </c>
       <c r="V25" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W25" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="X25" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="AD25">
         <v>307</v>
@@ -1770,19 +1653,16 @@
       <c r="AE25">
         <v>307</v>
       </c>
-      <c r="AG25">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="G26">
         <v>401</v>
@@ -1791,22 +1671,22 @@
         <v>401</v>
       </c>
       <c r="L26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="R26">
         <v>202</v>
@@ -1815,27 +1695,27 @@
         <v>202</v>
       </c>
       <c r="U26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="AA26">
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="G27">
         <v>203</v>
@@ -1844,28 +1724,28 @@
         <v>204</v>
       </c>
       <c r="I27" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="J27" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K27" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L27" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M27" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N27" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O27" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="P27" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V27">
         <v>302</v>
@@ -1877,86 +1757,86 @@
         <v>302</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>301</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="F28" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="H28">
         <v>301</v>
       </c>
       <c r="O28" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="P28" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="R28" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="V28" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W28">
         <v>308</v>
       </c>
       <c r="X28" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="AB28" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="AD28">
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="G29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="H29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="R29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="S29" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W29">
         <v>202</v>
@@ -1965,50 +1845,32 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="AA30" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="AC30" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="AD30" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="AE30" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF30" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG30" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI30" t="s">
-        <v>113</v>
-      </c>
-      <c r="AJ30" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK30" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="G31">
         <v>401</v>
@@ -2017,31 +1879,31 @@
         <v>401</v>
       </c>
       <c r="L31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="R31" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="S31" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="U31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V31">
         <v>203</v>
@@ -2050,7 +1912,7 @@
         <v>203</v>
       </c>
       <c r="X31" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y31">
         <v>301</v>
@@ -2068,36 +1930,24 @@
         <v>308</v>
       </c>
       <c r="AE31" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF31">
-        <v>302</v>
-      </c>
-      <c r="AG31">
-        <v>303</v>
-      </c>
-      <c r="AH31">
-        <v>307</v>
-      </c>
-      <c r="AI31">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="T32" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="X32" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y32" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Z32" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="AA32">
         <v>307</v>
@@ -2111,34 +1961,22 @@
       <c r="AE32">
         <v>307</v>
       </c>
-      <c r="AG32">
-        <v>308</v>
-      </c>
-      <c r="AH32">
-        <v>308</v>
-      </c>
-      <c r="AJ32">
-        <v>308</v>
-      </c>
-      <c r="AK32">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="J33" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K33" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L33" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M33" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V33">
         <v>304</v>
@@ -2153,42 +1991,33 @@
         <v>304</v>
       </c>
       <c r="AC33" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="AE33" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF33" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG33" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="L34" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="T34" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="U34" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="V34" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W34" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="X34">
         <v>307</v>
@@ -2200,7 +2029,7 @@
         <v>307</v>
       </c>
       <c r="AB34" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="AC34">
         <v>304</v>
@@ -2211,64 +2040,37 @@
       <c r="AE34">
         <v>306</v>
       </c>
-      <c r="AF34">
-        <v>304</v>
-      </c>
-      <c r="AH34">
-        <v>304</v>
-      </c>
-      <c r="AI34">
-        <v>305</v>
-      </c>
-      <c r="AJ34">
-        <v>306</v>
-      </c>
-      <c r="AK34">
-        <v>304</v>
-      </c>
-      <c r="AM34">
-        <v>304</v>
-      </c>
-      <c r="AN34">
-        <v>305</v>
-      </c>
-      <c r="AO34">
-        <v>306</v>
-      </c>
-      <c r="AP34">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="H35" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="L35" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="N35" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="O35" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="P35">
         <v>301</v>
       </c>
       <c r="T35" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="V35" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W35">
         <v>303</v>
@@ -2277,67 +2079,67 @@
         <v>303</v>
       </c>
       <c r="Z35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="B36">
         <v>301</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="H36">
         <v>301</v>
       </c>
       <c r="P36" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="V36" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="W36">
         <v>307</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="M37" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N37" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O37" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P37" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q37" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="R37" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C38">
         <v>307</v>
       </c>
       <c r="F38" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="G38">
         <v>307</v>
@@ -2349,65 +2151,62 @@
         <v>307</v>
       </c>
       <c r="S38" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="V38" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W38" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="X38" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y38" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Z38" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="AA38" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="AB38">
         <v>308</v>
       </c>
       <c r="AC38" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="AD38" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="AE38">
         <v>308</v>
       </c>
-      <c r="AF38">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="J39" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K39" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="L39" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M39" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="G40">
         <v>204</v>
@@ -2416,16 +2215,16 @@
         <v>204</v>
       </c>
       <c r="L40" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M40" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N40" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O40" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Y40">
         <v>109</v>
@@ -2440,15 +2239,15 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="G41">
         <v>204</v>
@@ -2457,137 +2256,89 @@
         <v>204</v>
       </c>
       <c r="L41" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="M41" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="N41" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O41" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="P41" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="B42">
         <v>302</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="D42" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="H42" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="J42" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="L42" t="s">
-        <v>101</v>
+        <v>69</v>
+      </c>
+      <c r="M42" t="s">
+        <v>69</v>
       </c>
       <c r="O42" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="P42" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="R42" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="S42" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="T42" t="s">
-        <v>101</v>
-      </c>
-      <c r="V42" t="s">
-        <v>101</v>
-      </c>
-      <c r="W42" t="s">
-        <v>96</v>
-      </c>
-      <c r="X42" t="s">
-        <v>101</v>
+        <v>69</v>
+      </c>
+      <c r="U42" t="s">
+        <v>69</v>
+      </c>
+      <c r="W42">
+        <v>307</v>
       </c>
       <c r="Y42" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="Z42" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA42" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB42">
-        <v>304</v>
+        <v>67</v>
       </c>
       <c r="AC42" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="AE42">
         <v>304</v>
       </c>
-      <c r="AF42">
-        <v>305</v>
-      </c>
-      <c r="AG42">
-        <v>306</v>
-      </c>
-      <c r="AH42">
-        <v>304</v>
-      </c>
-      <c r="AI42">
-        <v>303</v>
-      </c>
-      <c r="AK42">
-        <v>304</v>
-      </c>
-      <c r="AL42">
-        <v>305</v>
-      </c>
-      <c r="AM42">
-        <v>306</v>
-      </c>
-      <c r="AN42">
-        <v>304</v>
-      </c>
-      <c r="AO42">
-        <v>303</v>
-      </c>
-      <c r="AQ42">
-        <v>304</v>
-      </c>
-      <c r="AR42">
-        <v>305</v>
-      </c>
-      <c r="AS42">
-        <v>306</v>
-      </c>
-      <c r="AT42">
-        <v>304</v>
-      </c>
-      <c r="AU42">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B43">
         <v>203</v>
@@ -2608,16 +2359,16 @@
         <v>308</v>
       </c>
       <c r="N43" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="O43" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="R43" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="S43" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="U43">
         <v>301</v>
@@ -2647,33 +2398,18 @@
         <v>307</v>
       </c>
       <c r="AE43" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG43" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH43" t="s">
-        <v>96</v>
-      </c>
-      <c r="AI43">
-        <v>303</v>
-      </c>
-      <c r="AJ43">
-        <v>303</v>
-      </c>
-      <c r="AL43">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="J44" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K44" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="U44">
         <v>304</v>
@@ -2694,24 +2430,15 @@
         <v>306</v>
       </c>
       <c r="AC44" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="AE44" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF44" t="s">
-        <v>111</v>
-      </c>
-      <c r="AG44" t="s">
-        <v>111</v>
-      </c>
-      <c r="AH44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="I45">
         <v>302</v>
@@ -2723,9 +2450,9 @@
         <v>302</v>
       </c>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="I46">
         <v>307</v>
@@ -2734,9 +2461,9 @@
         <v>307</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="I47">
         <v>307</v>
@@ -2745,20 +2472,20 @@
         <v>307</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="J48" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="K48" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="X49">
         <v>306</v>
@@ -2775,7 +2502,7 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="X50">
         <v>309</v>
@@ -2787,15 +2514,15 @@
         <v>309</v>
       </c>
       <c r="AB50" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="AC50" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="B51">
         <v>203</v>
@@ -2810,7 +2537,7 @@
         <v>401</v>
       </c>
       <c r="L51" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>